<commit_message>
1. Edit Dokumentasi hasil uji coba.xlsx
</commit_message>
<xml_diff>
--- a/arithmetic_n/Dokumentasi hasil uji coba.xlsx
+++ b/arithmetic_n/Dokumentasi hasil uji coba.xlsx
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Original file</t>
-  </si>
-  <si>
-    <t>Size</t>
   </si>
   <si>
     <t>Compressed File</t>
@@ -42,6 +39,12 @@
   </si>
   <si>
     <t>ARITHMETIC_N CODING</t>
+  </si>
+  <si>
+    <t>Size (byte)</t>
+  </si>
+  <si>
+    <t>berk.raw</t>
   </si>
 </sst>
 </file>
@@ -85,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -94,6 +97,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -379,147 +388,316 @@
   <dimension ref="B2:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>1</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1151150</v>
+      </c>
+      <c r="E5" s="3" t="str">
+        <f>CONCATENATE(C5,".arith_n")</f>
+        <v>berk.raw.arith_n</v>
+      </c>
+      <c r="F5" s="3">
+        <v>2047514</v>
+      </c>
+      <c r="G5" s="5">
+        <v>-0.77</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>2</v>
       </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3" t="str">
+        <f t="shared" ref="E6:E24" si="0">CONCATENATE(C6,".arith_n")</f>
+        <v>.arith_n</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>3</v>
       </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>4</v>
       </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>5</v>
       </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>6</v>
       </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>7</v>
       </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>8</v>
       </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>9</v>
       </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>10</v>
       </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>11</v>
       </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>20</v>
       </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>.arith_n</v>
+      </c>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>